<commit_message>
Corrección archivos jornada 4 y 5, error Puche
</commit_message>
<xml_diff>
--- a/data/clasf_jor5_gA.xlsx
+++ b/data/clasf_jor5_gA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,212 +434,230 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Equipos</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Nºs 1º</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Max.pts</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>PJ</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Palop</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>10</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>44</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>3</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Ruso</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
       <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
         <v>51</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>3</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Kero</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>7</v>
       </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
       <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
         <v>50</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Tony</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>41</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Fale</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>6</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>37</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>2</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>3</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Lope</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>4</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>42</v>
       </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>3</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
       <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección columna posición de las clasificaciones
</commit_message>
<xml_diff>
--- a/data/clasf_jor5_gA.xlsx
+++ b/data/clasf_jor5_gA.xlsx
@@ -477,7 +477,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -570,7 +570,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -632,7 +632,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>

</xml_diff>